<commit_message>
QuadPipe Nova STD/HT MGN12 Added
</commit_message>
<xml_diff>
--- a/docs/Gear Ratio.xlsx
+++ b/docs/Gear Ratio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACC4520-74B8-47A3-B422-3E169FB9404D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601FAF02-0236-4A90-A70D-D75B0D20101A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E4242A01-2A35-4B13-A72D-C70EF3545C67}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{E4242A01-2A35-4B13-A72D-C70EF3545C67}"/>
   </bookViews>
   <sheets>
     <sheet name="ComparoGearing" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>BMG</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>mm/motorRev</t>
+  </si>
+  <si>
+    <t>HextrudORT_17</t>
   </si>
 </sst>
 </file>
@@ -241,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -265,6 +268,7 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,28 +588,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F3B8D7-A08F-4CB9-B1DD-94BFEB00D33A}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="10" max="10" width="20.1796875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -640,7 +644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -682,7 +686,7 @@
         <v>147.98554049664</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -723,7 +727,7 @@
         <v>88.662360863999993</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -763,6 +767,48 @@
       <c r="K4" s="10">
         <f t="shared" si="2"/>
         <v>87.050317939200013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5">
+        <v>50</v>
+      </c>
+      <c r="C5" s="5">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5">
+        <f>B5/C5</f>
+        <v>2.9411764705882355</v>
+      </c>
+      <c r="E5" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="F5" s="5">
+        <f>E5*3.1416</f>
+        <v>22.619520000000001</v>
+      </c>
+      <c r="G5" s="5">
+        <f>1/F5</f>
+        <v>4.4209603033132441E-2</v>
+      </c>
+      <c r="H5" s="5">
+        <f>G5*D5</f>
+        <v>0.13002824421509543</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" ref="I5" si="6">F5/D5</f>
+        <v>7.6906368000000001</v>
+      </c>
+      <c r="J5" s="6">
+        <f>H5*200*16</f>
+        <v>416.09038148830535</v>
+      </c>
+      <c r="K5" s="6">
+        <f>1/H5*(1.75/2)*(1.75/2)*3.1416*8</f>
+        <v>147.98554049664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added NF Cannon from Mellow
</commit_message>
<xml_diff>
--- a/docs/Gear Ratio.xlsx
+++ b/docs/Gear Ratio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601FAF02-0236-4A90-A70D-D75B0D20101A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2840518-94DC-4E06-9847-1107BC62E184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{E4242A01-2A35-4B13-A72D-C70EF3545C67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E4242A01-2A35-4B13-A72D-C70EF3545C67}"/>
   </bookViews>
   <sheets>
     <sheet name="ComparoGearing" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>BMG</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>HextrudORT_17</t>
+  </si>
+  <si>
+    <t>Hemera</t>
+  </si>
+  <si>
+    <t>Mellow NF Cannon</t>
   </si>
 </sst>
 </file>
@@ -244,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -269,6 +275,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,28 +596,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F3B8D7-A08F-4CB9-B1DD-94BFEB00D33A}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.26953125" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
-    <col min="10" max="10" width="20.1796875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -644,7 +650,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -661,32 +667,32 @@
       <c r="E2" s="5">
         <v>7.2</v>
       </c>
-      <c r="F2" s="5">
-        <f>E2*3.1416</f>
-        <v>22.619520000000001</v>
+      <c r="F2" s="11">
+        <f t="shared" ref="F2:F5" si="0">E2*PI()</f>
+        <v>22.61946710584651</v>
       </c>
       <c r="G2" s="5">
         <f>1/F2</f>
-        <v>4.4209603033132441E-2</v>
+        <v>4.4209706414415371E-2</v>
       </c>
       <c r="H2" s="5">
         <f>G2*D2</f>
-        <v>0.13002824421509543</v>
+        <v>0.13002854827769228</v>
       </c>
       <c r="I2" s="7">
-        <f t="shared" ref="I2:I3" si="0">F2/D2</f>
-        <v>7.6906368000000001</v>
+        <f t="shared" ref="I2:I3" si="1">F2/D2</f>
+        <v>7.6906188159878131</v>
       </c>
       <c r="J2" s="6">
         <f>H2*200*16</f>
-        <v>416.09038148830535</v>
+        <v>416.09135448861531</v>
       </c>
       <c r="K2" s="6">
         <f>1/H2*(1.75/2)*(1.75/2)*3.1416*8</f>
-        <v>147.98554049664</v>
+        <v>147.98519444288232</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -702,32 +708,32 @@
       <c r="E3" s="5">
         <v>11</v>
       </c>
-      <c r="F3" s="5">
-        <f t="shared" ref="F3:F4" si="1">E3*3.1416</f>
-        <v>34.557600000000001</v>
+      <c r="F3" s="11">
+        <f t="shared" si="0"/>
+        <v>34.557519189487721</v>
       </c>
       <c r="G3" s="5">
         <f>1/F3</f>
-        <v>2.893719471259578E-2</v>
+        <v>2.8937262380344612E-2</v>
       </c>
       <c r="H3" s="5">
         <f>G3*D3</f>
-        <v>0.21702896034446836</v>
+        <v>0.21702946785258459</v>
       </c>
       <c r="I3" s="9">
-        <f t="shared" si="0"/>
-        <v>4.6076800000000002</v>
+        <f t="shared" si="1"/>
+        <v>4.6076692252650293</v>
       </c>
       <c r="J3" s="6">
         <f>H3*200*16</f>
-        <v>694.4926731022988</v>
+        <v>694.49429712827066</v>
       </c>
       <c r="K3" s="6">
         <f t="shared" ref="K3:K4" si="2">1/H3*(1.75/2)*(1.75/2)*3.1416*8</f>
-        <v>88.662360863999993</v>
+        <v>88.662153533317266</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -744,32 +750,32 @@
       <c r="E4" s="7">
         <v>7.2</v>
       </c>
-      <c r="F4" s="7">
-        <f t="shared" si="1"/>
-        <v>22.619520000000001</v>
+      <c r="F4" s="11">
+        <f t="shared" si="0"/>
+        <v>22.61946710584651</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" ref="G4" si="3">1/F4</f>
-        <v>4.4209603033132441E-2</v>
+        <v>4.4209706414415371E-2</v>
       </c>
       <c r="H4" s="7">
         <f t="shared" ref="H4" si="4">G4*D4</f>
-        <v>0.22104801516566219</v>
+        <v>0.22104853207207686</v>
       </c>
       <c r="I4" s="9">
         <f>F4/D4</f>
-        <v>4.5239039999999999</v>
+        <v>4.5238934211693023</v>
       </c>
       <c r="J4" s="10">
         <f t="shared" ref="J4" si="5">H4*200*16</f>
-        <v>707.35364853011902</v>
+        <v>707.35530263064595</v>
       </c>
       <c r="K4" s="10">
         <f t="shared" si="2"/>
-        <v>87.050317939200013</v>
+        <v>87.050114378166072</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
@@ -786,29 +792,108 @@
       <c r="E5" s="5">
         <v>7.2</v>
       </c>
-      <c r="F5" s="5">
-        <f>E5*3.1416</f>
-        <v>22.619520000000001</v>
+      <c r="F5" s="11">
+        <f t="shared" si="0"/>
+        <v>22.61946710584651</v>
       </c>
       <c r="G5" s="5">
         <f>1/F5</f>
-        <v>4.4209603033132441E-2</v>
+        <v>4.4209706414415371E-2</v>
       </c>
       <c r="H5" s="5">
         <f>G5*D5</f>
-        <v>0.13002824421509543</v>
+        <v>0.13002854827769228</v>
       </c>
       <c r="I5" s="7">
-        <f t="shared" ref="I5" si="6">F5/D5</f>
-        <v>7.6906368000000001</v>
+        <f t="shared" ref="I5:I7" si="6">F5/D5</f>
+        <v>7.6906188159878131</v>
       </c>
       <c r="J5" s="6">
         <f>H5*200*16</f>
-        <v>416.09038148830535</v>
+        <v>416.09135448861531</v>
       </c>
       <c r="K5" s="6">
         <f>1/H5*(1.75/2)*(1.75/2)*3.1416*8</f>
-        <v>147.98554049664</v>
+        <v>147.98519444288232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5">
+        <v>3.32</v>
+      </c>
+      <c r="E6" s="11">
+        <v>8.27</v>
+      </c>
+      <c r="F6" s="11">
+        <f>E6*PI()</f>
+        <v>25.980971245187586</v>
+      </c>
+      <c r="G6" s="11">
+        <f>1/F6</f>
+        <v>3.8489708123795735E-2</v>
+      </c>
+      <c r="H6" s="5">
+        <f>G6*D6</f>
+        <v>0.12778583097100182</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="6"/>
+        <v>7.8255937485504781</v>
+      </c>
+      <c r="J6" s="6">
+        <f>H6*200*16</f>
+        <v>408.91465910720581</v>
+      </c>
+      <c r="K6" s="6">
+        <f>1/H6*(1.75/2)*(1.75/2)*3.1416*8</f>
+        <v>150.58242258773288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="12">
+        <v>39</v>
+      </c>
+      <c r="C7" s="12">
+        <v>2</v>
+      </c>
+      <c r="D7" s="13">
+        <f>B7/C7</f>
+        <v>19.5</v>
+      </c>
+      <c r="E7" s="13">
+        <v>18.8</v>
+      </c>
+      <c r="F7" s="12">
+        <f>E7*PI()</f>
+        <v>59.061941887488111</v>
+      </c>
+      <c r="G7" s="12">
+        <f>1/F7</f>
+        <v>1.6931376924669717E-2</v>
+      </c>
+      <c r="H7" s="13">
+        <f>G7*D7</f>
+        <v>0.33016185003105947</v>
+      </c>
+      <c r="I7" s="13">
+        <f t="shared" si="6"/>
+        <v>3.028817532691698</v>
+      </c>
+      <c r="J7" s="10">
+        <f>H7*200*16</f>
+        <v>1056.5179200993903</v>
+      </c>
+      <c r="K7" s="10">
+        <f>1/H7*(1.75/2)*(1.75/2)*3.1416*8</f>
+        <v>58.281415609313456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>